<commit_message>
feat: Change the lottery content in the config files from Chinese to English.
</commit_message>
<xml_diff>
--- a/server/data/users.xlsx
+++ b/server/data/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ynsong/Desktop/repos/lottery/server/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42D33A0-4677-954F-940C-947F47E9130C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E44F0D-D365-9140-A655-3D79A10C0802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1120" yWindow="500" windowWidth="32480" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t>姓名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -305,9 +305,6 @@
   <si>
     <t>Keith Zubchevich</t>
     <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Swaraj Yadav</t>
   </si>
   <si>
     <t>序号</t>
@@ -731,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B89"/>
+  <dimension ref="A1:B88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.6640625" defaultRowHeight="18"/>
@@ -744,7 +741,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1444,14 +1441,6 @@
       </c>
       <c r="B88" s="5" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2">
-      <c r="A89" s="2">
-        <v>88</v>
-      </c>
-      <c r="B89" s="5" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>